<commit_message>
Create a new 'Net exports' indicator and update the plots
</commit_message>
<xml_diff>
--- a/plots/summary_statistics.xlsx
+++ b/plots/summary_statistics.xlsx
@@ -154,8 +154,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -521,7 +521,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,273 +604,205 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>East Asia &amp; Pacific</t>
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>46844.26</v>
+        <v>6958.67</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>-0.44</v>
+        <v>0.25</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>-0.88</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>1068951450000</v>
+        <v>-1.53</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>15128517200000</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>-0.46</v>
+        <v>0.32</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>-1.13</v>
+        <v>-1.46</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>2.46</v>
+        <v>3</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>0.51</v>
+        <v>1.32</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>-0.26</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Central Europe and the Baltics</t>
+          <t>Europe &amp; Central Asia</t>
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>11741.85</v>
+        <v>20157.45</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>-0.73</v>
+        <v>-0.47</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>-0.66</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>1222242750000</v>
+        <v>-1.44</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>17540027200000</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>-0.82</v>
+        <v>-0.47</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>-0.53</v>
+        <v>-1.47</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>2.76</v>
+        <v>2.89</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>0.06</v>
+        <v>1.09</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>-0.31</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>East Asia &amp; Pacific</t>
+          <t>Latin America &amp; Caribbean</t>
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>7729.5</v>
+        <v>6913.53</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>-0.12</v>
+        <v>0.04</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>-1.47</v>
+        <v>-1.54</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>16997744500000</v>
+        <v>4067189600000</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>-0.02</v>
+        <v>0.04</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>-1.46</v>
+        <v>-1.63</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>2.83</v>
+        <v>3.88</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>1.75</v>
+        <v>0.71</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>3.81</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Latin America &amp; Caribbean</t>
+          <t>Middle East &amp; North Africa</t>
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>7551.67</v>
+        <v>5733.24</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>-0.44</v>
+        <v>-0.18</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>-1.12</v>
+        <v>-1.59</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>4526825000000</v>
+        <v>2018788800000</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>-0.43</v>
+        <v>0.01</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>-1.25</v>
+        <v>-1.73</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>3.47</v>
+        <v>3.02</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>1.05</v>
+        <v>2.81</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>1.96</v>
+        <v>9.550000000000001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Middle East &amp; North Africa</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>6422.83</v>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>46319.07</v>
       </c>
       <c r="C8" s="3" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>-1.17</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>16274864400000</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>-1.15</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="I8" s="3" t="n">
         <v>-0.66</v>
       </c>
-      <c r="D8" s="3" t="n">
-        <v>-0.89</v>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>2318333150000</v>
-      </c>
-      <c r="F8" s="3" t="n">
-        <v>-0.43</v>
-      </c>
-      <c r="G8" s="3" t="n">
-        <v>-1.43</v>
-      </c>
-      <c r="H8" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="I8" s="3" t="n">
-        <v>2.7</v>
-      </c>
       <c r="J8" s="3" t="n">
-        <v>8.02</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Sub-Saharan Africa</t>
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>49909.12</v>
+        <v>1259.2</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>-0.12</v>
+        <v>-0.23</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>-0.95</v>
+        <v>-1.52</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>17851815000000</v>
+        <v>1135243880000</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>-0.05</v>
+        <v>-0.08</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>-0.97</v>
+        <v>-1.66</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>1.95</v>
+        <v>5.49</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>-0.68</v>
+        <v>0.95</v>
       </c>
       <c r="J9" s="3" t="n">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>South Asia</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="n">
-        <v>1201.19</v>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>-0</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>-1.29</v>
-      </c>
-      <c r="E10" s="3" t="n">
-        <v>2162981500000</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="G10" s="3" t="n">
-        <v>-1.24</v>
-      </c>
-      <c r="H10" s="5" t="n">
-        <v>5.92</v>
-      </c>
-      <c r="I10" s="3" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="J10" s="3" t="n">
-        <v>-0.64</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>Sub-Saharan Africa</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="n">
-        <v>1415.13</v>
-      </c>
-      <c r="C11" s="3" t="n">
-        <v>-0.77</v>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>-0.54</v>
-      </c>
-      <c r="E11" s="3" t="n">
-        <v>1317853200000</v>
-      </c>
-      <c r="F11" s="3" t="n">
-        <v>-0.53</v>
-      </c>
-      <c r="G11" s="3" t="n">
-        <v>-1.19</v>
-      </c>
-      <c r="H11" s="3" t="n">
-        <v>5.36</v>
-      </c>
-      <c r="I11" s="3" t="n">
-        <v>1.22</v>
-      </c>
-      <c r="J11" s="3" t="n">
-        <v>2.07</v>
+        <v>1.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replace the statsmodule with scipy, increase the font size of the text in the heatmap, and clean up the code
</commit_message>
<xml_diff>
--- a/plots/summary_statistics.xlsx
+++ b/plots/summary_statistics.xlsx
@@ -547,7 +547,7 @@
       <c r="G1" s="2" t="n"/>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Inflation, consumer prices (annual %)</t>
+          <t>Net migration</t>
         </is>
       </c>
       <c r="I1" s="2" t="n"/>
@@ -626,13 +626,13 @@
         <v>-1.46</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>3</v>
+        <v>-29158.12</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1.32</v>
+        <v>0.19</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>1.92</v>
+        <v>-1.43</v>
       </c>
     </row>
     <row r="5">
@@ -660,13 +660,13 @@
         <v>-1.47</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>2.89</v>
+        <v>1099373.6</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>1.09</v>
+        <v>-1.11</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>1.27</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="6">
@@ -693,14 +693,14 @@
       <c r="G6" s="3" t="n">
         <v>-1.63</v>
       </c>
-      <c r="H6" s="3" t="n">
-        <v>3.88</v>
+      <c r="H6" s="5" t="n">
+        <v>-698788.4399999999</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>0.71</v>
+        <v>0.45</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>0.24</v>
+        <v>-1.19</v>
       </c>
     </row>
     <row r="7">
@@ -728,13 +728,13 @@
         <v>-1.73</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>3.02</v>
+        <v>409604.44</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>2.81</v>
+        <v>-0.21</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>9.550000000000001</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="8">
@@ -761,14 +761,14 @@
       <c r="G8" s="3" t="n">
         <v>-1.15</v>
       </c>
-      <c r="H8" s="5" t="n">
-        <v>1.98</v>
+      <c r="H8" s="4" t="n">
+        <v>1515907.4</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>-0.66</v>
+        <v>-0.09</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>0.16</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9">
@@ -795,14 +795,14 @@
       <c r="G9" s="3" t="n">
         <v>-1.66</v>
       </c>
-      <c r="H9" s="4" t="n">
-        <v>5.49</v>
+      <c r="H9" s="3" t="n">
+        <v>-539396.36</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>0.95</v>
+        <v>0.35</v>
       </c>
       <c r="J9" s="3" t="n">
-        <v>1.25</v>
+        <v>1.73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>